<commit_message>
Updated temp lmer results
</commit_message>
<xml_diff>
--- a/results/Temp Results/lmer_ind_effects_m1_basin_season_temp.xlsx
+++ b/results/Temp Results/lmer_ind_effects_m1_basin_season_temp.xlsx
@@ -53,13 +53,19 @@
     <t xml:space="preserve">fish_basinNorth</t>
   </si>
   <si>
+    <t xml:space="preserve">seasonSpring</t>
+  </si>
+  <si>
     <t xml:space="preserve">seasonSummer</t>
   </si>
   <si>
     <t xml:space="preserve">seasonFall</t>
   </si>
   <si>
-    <t xml:space="preserve">seasonWinter</t>
+    <t xml:space="preserve">fish_basinWest:seasonSpring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fish_basinNorth:seasonSpring</t>
   </si>
   <si>
     <t xml:space="preserve">fish_basinWest:seasonSummer</t>
@@ -72,12 +78,6 @@
   </si>
   <si>
     <t xml:space="preserve">fish_basinNorth:seasonFall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fish_basinWest:seasonWinter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fish_basinNorth:seasonWinter</t>
   </si>
   <si>
     <t xml:space="preserve">ran_pars</t>
@@ -459,16 +459,16 @@
         <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>1.38408124217894</v>
+        <v>0.890273349211537</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0368791373970953</v>
+        <v>0.0368068944451756</v>
       </c>
       <c r="G2" t="n">
-        <v>37.5301956571238</v>
+        <v>24.1876790376219</v>
       </c>
       <c r="H2" t="n">
-        <v>0</v>
+        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000000299885823158512</v>
       </c>
     </row>
     <row r="3">
@@ -483,16 +483,16 @@
         <v>11</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0642974546029044</v>
+        <v>0.0855718387729713</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0461584814777494</v>
+        <v>0.0462083381610194</v>
       </c>
       <c r="G3" t="n">
-        <v>1.39297161744584</v>
+        <v>1.85187007753415</v>
       </c>
       <c r="H3" t="n">
-        <v>0.163628373638613</v>
+        <v>0.0640444816511403</v>
       </c>
     </row>
     <row r="4">
@@ -507,16 +507,16 @@
         <v>12</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0528388240821225</v>
+        <v>0.326839706197089</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0568805774239297</v>
+        <v>0.0568589075625431</v>
       </c>
       <c r="G4" t="n">
-        <v>0.928943173138273</v>
+        <v>5.74825863190521</v>
       </c>
       <c r="H4" t="n">
-        <v>0.352918537207765</v>
+        <v>0.00000000901672445966544</v>
       </c>
     </row>
     <row r="5">
@@ -531,16 +531,16 @@
         <v>13</v>
       </c>
       <c r="E5" t="n">
-        <v>0.712794326582018</v>
+        <v>0.493774947317767</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0134906174806111</v>
+        <v>0.0137327213317911</v>
       </c>
       <c r="G5" t="n">
-        <v>52.8363010519315</v>
+        <v>35.9560887742391</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>4.06559277235843e-283</v>
       </c>
     </row>
     <row r="6">
@@ -555,13 +555,13 @@
         <v>14</v>
       </c>
       <c r="E6" t="n">
-        <v>0.634206717711025</v>
+        <v>1.20658634091772</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0133975003575999</v>
+        <v>0.013593949360044</v>
       </c>
       <c r="G6" t="n">
-        <v>47.3376899259618</v>
+        <v>88.7590728022113</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
@@ -579,16 +579,16 @@
         <v>15</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.493787367826652</v>
+        <v>1.1279933706489</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0137327662130015</v>
+        <v>0.0132717258152763</v>
       </c>
       <c r="G7" t="n">
-        <v>-35.9568757064514</v>
+        <v>84.992214754055</v>
       </c>
       <c r="H7" t="n">
-        <v>3.95208145103122e-283</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -603,16 +603,16 @@
         <v>16</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.0255826569362931</v>
+        <v>-0.021232815987736</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0181624432942908</v>
+        <v>0.0186517741610287</v>
       </c>
       <c r="G8" t="n">
-        <v>-1.40854710579247</v>
+        <v>-1.13838049959345</v>
       </c>
       <c r="H8" t="n">
-        <v>0.15896912873756</v>
+        <v>0.254961633149316</v>
       </c>
     </row>
     <row r="9">
@@ -627,16 +627,16 @@
         <v>17</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.17615131498856</v>
+        <v>-0.273984351683324</v>
       </c>
       <c r="F9" t="n">
-        <v>0.022355743127259</v>
+        <v>0.0218687244996009</v>
       </c>
       <c r="G9" t="n">
-        <v>-7.87946587084254</v>
+        <v>-12.5285931371226</v>
       </c>
       <c r="H9" t="n">
-        <v>0.00000000000000328783482541017</v>
+        <v>0.00000000000000000000000000000000000520782920806283</v>
       </c>
     </row>
     <row r="10">
@@ -651,16 +651,16 @@
         <v>18</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.0609960156133606</v>
+        <v>-0.0468302195593423</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0178749153829287</v>
+        <v>0.0183477409328543</v>
       </c>
       <c r="G10" t="n">
-        <v>-3.41238066344158</v>
+        <v>-2.55236978387274</v>
       </c>
       <c r="H10" t="n">
-        <v>0.000643981165311461</v>
+        <v>0.0106992895461227</v>
       </c>
     </row>
     <row r="11">
@@ -675,16 +675,16 @@
         <v>19</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.114183571086671</v>
+        <v>-0.450130254304272</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0214272771606509</v>
+        <v>0.0224021836819427</v>
       </c>
       <c r="G11" t="n">
-        <v>-5.32888851115242</v>
+        <v>-20.0931418425561</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0000000988156286409392</v>
+        <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000000000000000847272504723124</v>
       </c>
     </row>
     <row r="12">
@@ -699,16 +699,16 @@
         <v>20</v>
       </c>
       <c r="E12" t="n">
-        <v>0.0212532291432624</v>
+        <v>-0.0822485260186274</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0186518181023392</v>
+        <v>0.0180131710045114</v>
       </c>
       <c r="G12" t="n">
-        <v>1.13947225019297</v>
+        <v>-4.5660214960502</v>
       </c>
       <c r="H12" t="n">
-        <v>0.25450623606101</v>
+        <v>0.00000497067818095543</v>
       </c>
     </row>
     <row r="13">
@@ -723,16 +723,16 @@
         <v>21</v>
       </c>
       <c r="E13" t="n">
-        <v>0.274003360955053</v>
+        <v>-0.388174676513601</v>
       </c>
       <c r="F13" t="n">
-        <v>0.021868820404409</v>
+        <v>0.0214361986366336</v>
       </c>
       <c r="G13" t="n">
-        <v>12.5294074343311</v>
+        <v>-18.1083728087044</v>
       </c>
       <c r="H13" t="n">
-        <v>0.00000000000000000000000000000000000515463644438451</v>
+        <v>0.000000000000000000000000000000000000000000000000000000000000000000000000273720259666219</v>
       </c>
     </row>
     <row r="14">
@@ -749,7 +749,7 @@
         <v>24</v>
       </c>
       <c r="E14" t="n">
-        <v>0.0867974807366187</v>
+        <v>0.0867992057914639</v>
       </c>
       <c r="F14"/>
       <c r="G14"/>
@@ -769,7 +769,7 @@
         <v>24</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0255542550767551</v>
+        <v>0.0255597934641572</v>
       </c>
       <c r="F15"/>
       <c r="G15"/>

</xml_diff>